<commit_message>
Started on returning function result with all params constant
</commit_message>
<xml_diff>
--- a/Test data/Multi-x/DataSet2.xlsx
+++ b/Test data/Multi-x/DataSet2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marietje\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marietje\git\Blits\Test data\Multi-x\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,11 +352,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,7 +377,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.0000000000000001E-15</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>67.640139322431423</v>

</xml_diff>